<commit_message>
added picture link to readme
</commit_message>
<xml_diff>
--- a/data/category_seperation.xlsx
+++ b/data/category_seperation.xlsx
@@ -295,14 +295,14 @@
   </sheetPr>
   <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G20" activeCellId="0" sqref="G20"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G32" activeCellId="0" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.3805668016194"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.4939271255061"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -879,7 +879,7 @@
         <v>47.4481437813987</v>
       </c>
       <c r="E34" s="0" t="n">
-        <v>188</v>
+        <v>18</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>